<commit_message>
ajout nouveaux produit + fusion fichiers xls
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiphaine\Documents\scraping_eaugo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiphaine\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820B308D-5C70-4FA4-8107-4B56AC68FA30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD53B65-9E14-42E4-BDF6-DAC8C13F9BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{C411A034-5389-4F96-8ECE-DDB492652C9E}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="cdes et cout" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'produits à surveiller'!$A$1:$S$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'produits à surveiller'!$A$1:$H$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="390">
   <si>
     <t>154330-l</t>
   </si>
@@ -589,27 +589,6 @@
     <t>Cde ls 2020</t>
   </si>
   <si>
-    <t>chauffe-eau</t>
-  </si>
-  <si>
-    <t>FR:::0</t>
-  </si>
-  <si>
-    <t>Blanc</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>DE DIETRICH</t>
-  </si>
-  <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-200l-de-dietrich-ceb-vertical-mural-407.html</t>
-  </si>
-  <si>
     <t>en stock</t>
   </si>
   <si>
@@ -631,9 +610,6 @@
     <t>https://www.eau-go.fr/3337-home_default/chauffe-eau-electrique-150l-de-dietrich-ceb-vertical-mural.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-150l-de-dietrich-ceb-vertical-mural-24.html</t>
-  </si>
-  <si>
     <t>238.00 €</t>
   </si>
   <si>
@@ -649,9 +625,6 @@
     <t>https://www.eau-go.fr/3336-home_default/chauffe-eau-electrique-100l-de-dietrich-ceb-vertical-mural.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-100l-de-dietrich-ceb-vertical-mural-23.html</t>
-  </si>
-  <si>
     <t>217.50 €</t>
   </si>
   <si>
@@ -664,15 +637,9 @@
     <t>89789651-L</t>
   </si>
   <si>
-    <t>THERMOR</t>
-  </si>
-  <si>
     <t>https://www.eau-go.fr/3332-home_default/chauffe-eau-electrique-150l-thermor-duralis-vertical-mural.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-150l-thermor-duralis-vertical-mural-123.html</t>
-  </si>
-  <si>
     <t>329.00 €</t>
   </si>
   <si>
@@ -688,9 +655,6 @@
     <t>https://www.eau-go.fr/3335-home_default/chauffe-eau-electrique-300l-de-dietrich-cor-email-ths-vertical-sur-socle.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-300l-de-dietrich-cor-email-ths-vertical-sur-socle-13.html</t>
-  </si>
-  <si>
     <t>590.00 €</t>
   </si>
   <si>
@@ -706,9 +670,6 @@
     <t>https://www.eau-go.fr/3329-home_default/chauffe-eau-electrique-300l-thermor-duralis-vertical-stable.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-300l-thermor-duralis-vertical-stable-39.html</t>
-  </si>
-  <si>
     <t>619.50 €</t>
   </si>
   <si>
@@ -724,9 +685,6 @@
     <t>https://www.eau-go.fr/3327-home_default/chauffe-eau-electrique-300l-thermor-steatis-stable.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-300l-thermor-steatis-stable-38.html</t>
-  </si>
-  <si>
     <t>503.90 €</t>
   </si>
   <si>
@@ -742,9 +700,6 @@
     <t>https://www.eau-go.fr/3325-home_default/chauffe-eau-electrique-250l-thermor-duralis-vertical-stable.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-250l-thermor-duralis-vertical-stable-36.html</t>
-  </si>
-  <si>
     <t>607.00 €</t>
   </si>
   <si>
@@ -760,9 +715,6 @@
     <t>https://www.eau-go.fr/3324-home_default/chauffe-eau-electrique-200l-thermor-duralis-vertical-stable.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-200l-thermor-duralis-vertical-stable-182.html</t>
-  </si>
-  <si>
     <t>599.00 €</t>
   </si>
   <si>
@@ -778,9 +730,6 @@
     <t>https://www.eau-go.fr/3322-home_default/chauffe-eau-electrique-200l-thermor-duralis-mural-vertical.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-200l-thermor-duralis-mural-vertical-34.html</t>
-  </si>
-  <si>
     <t>374.99 €</t>
   </si>
   <si>
@@ -799,9 +748,6 @@
     <t>https://www.eau-go.fr/3312-home_default/chauffe-eau-electrique-100l-thermor-blinde-vertical-mural.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-100l-thermor-blinde-vertical-mural-562.html</t>
-  </si>
-  <si>
     <t>200.90 €</t>
   </si>
   <si>
@@ -814,9 +760,6 @@
     <t>https://www.eau-go.fr/3311-home_default/chauffe-eau-electrique-100l-thermor-steatis-vertical-mural-livraison-gratuite.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-100l-thermor-steatis-vertical-mural-livraison-gratuite-193.html</t>
-  </si>
-  <si>
     <t>239.00 €</t>
   </si>
   <si>
@@ -826,15 +769,9 @@
     <t>261025-L</t>
   </si>
   <si>
-    <t>ATLANTIC</t>
-  </si>
-  <si>
     <t>https://www.eau-go.fr/3291-thickbox_default/chauffe-eau-electrique-300l-atlantic-vizengo-vertical.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-300l-atlantic-vizengo-vertical-sur-socle-114.html</t>
-  </si>
-  <si>
     <t>797.00 €</t>
   </si>
   <si>
@@ -847,9 +784,6 @@
     <t>https://www.eau-go.fr/3286-home_default/chauffe-eau-electrique-250l-atlantic-vizengo-vertical-sur-socle.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-250l-atlantic-vizengo-vertical-sur-socle-113.html</t>
-  </si>
-  <si>
     <t>765.80 €</t>
   </si>
   <si>
@@ -865,9 +799,6 @@
     <t>https://www.eau-go.fr/3288-thickbox_default/chauffe-eau-electrique-300l-atlantic-zeneo-vertical-sur-socle.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-300l-atlantic-zeneo-vertical-sur-socle-108.html</t>
-  </si>
-  <si>
     <t>636.00 €</t>
   </si>
   <si>
@@ -883,9 +814,6 @@
     <t>https://www.eau-go.fr/3287-thickbox_default/chauffe-eau-electrique-250l-atlantic-zeneo-vertical-sur-socle.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-250l-atlantic-zeneo-vertical-sur-socle-107.html</t>
-  </si>
-  <si>
     <t>601.00 €</t>
   </si>
   <si>
@@ -901,9 +829,6 @@
     <t>https://www.eau-go.fr/3284-thickbox_default/chauffe-eau-electrique-200l-atlantic-zeneo-vertical-sur-socle.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-200l-atlantic-zeneo-vertical-sur-socle-106.html</t>
-  </si>
-  <si>
     <t>609.00 €</t>
   </si>
   <si>
@@ -916,9 +841,6 @@
     <t>https://www.eau-go.fr/3303-thickbox_default/chauffe-eau-electrique-150l-atlantic-zeneo-vertical-sur-socle.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-150l-atlantic-zeneo-vertical-sur-socle-105.html</t>
-  </si>
-  <si>
     <t>545.90 €</t>
   </si>
   <si>
@@ -934,9 +856,6 @@
     <t>https://www.eau-go.fr/3282-thickbox_default/chauffe-eau-electrique-200l-atlantic-vizengo-vertical-mural.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-200l-atlantic-vizengo-vertical-mural-112.html</t>
-  </si>
-  <si>
     <t>506.70 €</t>
   </si>
   <si>
@@ -952,9 +871,6 @@
     <t>https://www.eau-go.fr/3302-home_default/chauffe-eau-electrique-150l-atlantic-vizengo-vertical-mural.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-150l-atlantic-vizengo-vertical-mural-111.html</t>
-  </si>
-  <si>
     <t>449.00 €</t>
   </si>
   <si>
@@ -970,9 +886,6 @@
     <t>https://www.eau-go.fr/3301-thickbox_default/chauffe-eau-electrique-200l-atlantic-zeneo-vertical-mural.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-200l-atlantic-zeneo-vertical-mural-104.html</t>
-  </si>
-  <si>
     <t>376.90 €</t>
   </si>
   <si>
@@ -985,9 +898,6 @@
     <t>https://www.eau-go.fr/3300-thickbox_default/chauffe-eau-electrique-150l-atlantic-zeneo-vertical-mural.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-150l-atlantic-zeneo-vertical-mural-530.html</t>
-  </si>
-  <si>
     <t>332.00 €</t>
   </si>
   <si>
@@ -1003,9 +913,6 @@
     <t>https://www.eau-go.fr/3343-home_default/chauffe-eau-electrique-200l-de-dietrich-cor-email-ths-vertical-mural.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-200l-de-dietrich-cor-email-ths-vertical-mural-10.html</t>
-  </si>
-  <si>
     <t>362.00€</t>
   </si>
   <si>
@@ -1021,9 +928,6 @@
     <t>https://www.eau-go.fr/3289-thickbox_default/chauffe-eau-electrique-300l-atlantic-chauffeo-plus-vertical-sur-socle.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-300l-atlantic-chauffeo-plus-vertical-sur-socle-506.html</t>
-  </si>
-  <si>
     <t>495.00 €</t>
   </si>
   <si>
@@ -1039,9 +943,6 @@
     <t>https://www.eau-go.fr/3281-home_default/chauffe-eau-electrique-200l-atlantic-chauffeo-plus-vertical-mural.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-200l-atlantic-chauffeo-plus-vertical-mural-515.html</t>
-  </si>
-  <si>
     <t>294.00 €</t>
   </si>
   <si>
@@ -1057,9 +958,6 @@
     <t>https://www.eau-go.fr/3298-thickbox_default/chauffe-eau-electrique-200l-atlantic-chauffeo-horizontal-sortie-basse.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-200l-atlantic-chauffeo-horizontal-sortie-basse-85.html</t>
-  </si>
-  <si>
     <t>466.00 €</t>
   </si>
   <si>
@@ -1075,9 +973,6 @@
     <t>https://www.eau-go.fr/3296-thickbox_default/chauffe-eau-electrique-150l-atlantic-chauffeo-horizontal-sortie-basse.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-150l-atlantic-chauffeo-horizontal-sortie-basse-84.html</t>
-  </si>
-  <si>
     <t>418.00 €</t>
   </si>
   <si>
@@ -1093,9 +988,6 @@
     <t>https://www.eau-go.fr/3295-home_default/chauffe-eau-electrique-100l-atlantic-100-chauffeo-horizontal-sortie-basse.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-100l-atlantic-100-chauffeo-horizontal-sortie-basse-83.html</t>
-  </si>
-  <si>
     <t>354.00€</t>
   </si>
   <si>
@@ -1111,9 +1003,6 @@
     <t>https://www.eau-go.fr/3294-thickbox_default/chauffe-eau-electrique-200l-atlantic-chauffeo-vertical-sur-socle.jpg</t>
   </si>
   <si>
-    <t>https://www.eau-go.fr/chauffe-eau-electrique-200l-atlantic-chauffeo-vertical-sur-socle-46.html</t>
-  </si>
-  <si>
     <t>411.00 €</t>
   </si>
   <si>
@@ -1126,42 +1015,12 @@
     <t>022120-L</t>
   </si>
   <si>
-    <t>custom_label_0</t>
-  </si>
-  <si>
-    <t>additional_image_link</t>
-  </si>
-  <si>
-    <t>shipping</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>adult</t>
-  </si>
-  <si>
-    <t>google_product_category</t>
-  </si>
-  <si>
-    <t>identifier_exist</t>
-  </si>
-  <si>
-    <t>brand</t>
-  </si>
-  <si>
-    <t>mpn</t>
-  </si>
-  <si>
     <t>gtin</t>
   </si>
   <si>
     <t>image_link</t>
   </si>
   <si>
-    <t>link</t>
-  </si>
-  <si>
     <t>availability</t>
   </si>
   <si>
@@ -1180,7 +1039,175 @@
     <t>id</t>
   </si>
   <si>
-    <t>volume</t>
+    <t>CHAUFFE-EAU ÉLECTRIQUE 300L ATLANTIC CHAUFFÉO VERTICAL SUR SOCLE LIVRÉ</t>
+  </si>
+  <si>
+    <t>231070-L</t>
+  </si>
+  <si>
+    <t>CHAUFFE-EAU ÉLECTRIQUE 80L THERMOR MALICIO 3 CONNECTÉ VERTICAL OU HORIZONTAL</t>
+  </si>
+  <si>
+    <t>153112-L</t>
+  </si>
+  <si>
+    <t>153109-L</t>
+  </si>
+  <si>
+    <t>153111-L</t>
+  </si>
+  <si>
+    <t>051015-L</t>
+  </si>
+  <si>
+    <t>CHAUFFE-EAU ÉLECTRIQUE 200L ATLANTIC ZÉNÉO VERTICAL MURAL</t>
+  </si>
+  <si>
+    <t>CHAUFFE-EAU ÉLECTRIQUE 100L ATLANTIC ZÉNÉO VERTICAL MURAL</t>
+  </si>
+  <si>
+    <t>CHAUFFE-EAU ÉLECTRIQUE 150L ATLANTIC ZÉNÉO VERTICAL MURAL</t>
+  </si>
+  <si>
+    <t>021114-L</t>
+  </si>
+  <si>
+    <t>CHAUFFE-EAU ÉLECTRIQUE 100L ATLANTIC CHAUFFÉO VERTICAL MURAL</t>
+  </si>
+  <si>
+    <t>CHAUFFE EAU ELECTRIQUE 150L ATLANTIC CHAUFFÉO PLUS VERTICAL MURAL LIVRÉ</t>
+  </si>
+  <si>
+    <t>CHAUFFE EAU ELECTRIQUE 150L ATLANTIC CHAUFFÉO PLUS VERTICAL MURAL</t>
+  </si>
+  <si>
+    <t>053016-L</t>
+  </si>
+  <si>
+    <t>CHAUFFE-EAU ÉLECTRIQUE 200L ATLANTIC CHAUFFÉO PLUS VERTICAL MURAL</t>
+  </si>
+  <si>
+    <t>053017-L</t>
+  </si>
+  <si>
+    <t>22330-L</t>
+  </si>
+  <si>
+    <t>"1915956955424454498"</t>
+  </si>
+  <si>
+    <t>"2774528271263507905"</t>
+  </si>
+  <si>
+    <t>"2253125293629913071"</t>
+  </si>
+  <si>
+    <t>"14415108684127899091"</t>
+  </si>
+  <si>
+    <t>"1434101178178227170"</t>
+  </si>
+  <si>
+    <t>"14827813489941469003"</t>
+  </si>
+  <si>
+    <t>"1778678479788252976"</t>
+  </si>
+  <si>
+    <t>"8641869224973479543"</t>
+  </si>
+  <si>
+    <t>"5005337530000083532"</t>
+  </si>
+  <si>
+    <t>"3226561662642652118"</t>
+  </si>
+  <si>
+    <t>"12369944218821632914"</t>
+  </si>
+  <si>
+    <t>"18229353084856223101"</t>
+  </si>
+  <si>
+    <t>"3534764604662730729"</t>
+  </si>
+  <si>
+    <t>"5171588767110655760"</t>
+  </si>
+  <si>
+    <t>"4045238434942960469"</t>
+  </si>
+  <si>
+    <t>"11064213080907454068"</t>
+  </si>
+  <si>
+    <t>"5839687494743863490"</t>
+  </si>
+  <si>
+    <t>"13926597533192887454"</t>
+  </si>
+  <si>
+    <t>"1980162464924696186"</t>
+  </si>
+  <si>
+    <t>"138941720638156942"</t>
+  </si>
+  <si>
+    <t>"10848968015413876687"</t>
+  </si>
+  <si>
+    <t>"2989336499622483795"</t>
+  </si>
+  <si>
+    <t>"6264907038321286451"</t>
+  </si>
+  <si>
+    <t>"17357928556344687751"</t>
+  </si>
+  <si>
+    <t>"245389360969337290"</t>
+  </si>
+  <si>
+    <t>"10281122032644161409"</t>
+  </si>
+  <si>
+    <t>"17662283569304226148"</t>
+  </si>
+  <si>
+    <t>"10909035658102556437"</t>
+  </si>
+  <si>
+    <t>"6913732575834207279"</t>
+  </si>
+  <si>
+    <t>"16291017718281204086"</t>
+  </si>
+  <si>
+    <t>"3496036216085904968"</t>
+  </si>
+  <si>
+    <t>"157623965100331230"</t>
+  </si>
+  <si>
+    <t>"1778885318680457584"</t>
+  </si>
+  <si>
+    <t>"16579123116084811893"</t>
+  </si>
+  <si>
+    <t>"10427623138284075950"</t>
+  </si>
+  <si>
+    <t>"4782621681837071908"</t>
+  </si>
+  <si>
+    <t>google_shopping</t>
+  </si>
+  <si>
+    <t>"17733589981678581136"</t>
+  </si>
+  <si>
+    <t>"1912260605018180873"</t>
   </si>
 </sst>
 </file>
@@ -1188,9 +1215,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0&quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0&quot;€&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1220,8 +1247,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1232,12 +1265,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9CB9C"/>
-        <bgColor rgb="FFF9CB9C"/>
       </patternFill>
     </fill>
     <fill>
@@ -1258,6 +1285,18 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1272,7 +1311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1286,11 +1325,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -1301,9 +1337,9 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1311,12 +1347,16 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="1" fontId="1" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1637,1803 +1677,1070 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA940"/>
+  <dimension ref="A1:J940"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="14.41796875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="72.578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="66.83984375" style="6" customWidth="1"/>
-    <col min="5" max="7" width="14.41796875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="80.26171875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="113.83984375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="21.41796875" style="12" customWidth="1"/>
-    <col min="11" max="17" width="14.41796875" style="6"/>
-    <col min="18" max="18" width="25" style="6" customWidth="1"/>
-    <col min="19" max="27" width="35.83984375" style="6" customWidth="1"/>
-    <col min="28" max="16384" width="14.41796875" style="6"/>
+    <col min="1" max="1" width="11.41796875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="90.734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="66.83984375" style="6" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="6" width="14.41796875" style="6" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="113.83984375" style="6" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="21.41796875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="28.7890625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="25.578125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="14.41796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
-        <v>379</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>375</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>374</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>373</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>370</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>368</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>366</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-    </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="B2" s="13">
-        <f>VLOOKUP(A2,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>32.770000000000003</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="J2" s="15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="H2" s="12">
         <v>3410531543308</v>
       </c>
-      <c r="K2" s="13">
-        <v>154330</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M2" s="13" t="s">
+      <c r="I2" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="J2" s="23"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="H3" s="12">
+        <v>3410531544305</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="J3" s="23"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="N2" s="13">
-        <v>621</v>
-      </c>
-      <c r="O2" s="13" t="s">
+      <c r="C4" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="D4" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="E4" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13" t="s">
+      <c r="F4" s="17" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="B3" s="13">
-        <f>VLOOKUP(A3,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>15.09</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="J3" s="15">
-        <v>3410531544305</v>
-      </c>
-      <c r="K3" s="13">
-        <v>154430</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N3" s="13">
-        <v>621</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="B4" s="13">
-        <f>VLOOKUP(A4,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>12.5</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="I4" s="19" t="str">
+      <c r="G4" s="16" t="str">
         <f>HYPERLINK("https://www.eau-go.fr/3338-home_default/chauffe-eau-electrique-200l-de-dietrich-ceb-vertical-mural.jpg","https://www.eau-go.fr/3338-home_default/chauffe-eau-electrique-200l-de-dietrich-ceb-vertical-mural.jpg")</f>
         <v>https://www.eau-go.fr/3338-home_default/chauffe-eau-electrique-200l-de-dietrich-ceb-vertical-mural.jpg</v>
       </c>
-      <c r="J4" s="21">
+      <c r="H4" s="18">
         <v>3661238046573</v>
       </c>
-      <c r="K4" s="22">
-        <v>89789671</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="N4" s="22">
-        <v>621</v>
-      </c>
-      <c r="O4" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="P4" s="20" t="s">
+      <c r="I4" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J4" s="23"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="Q4" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20" t="s">
+      <c r="E5" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="13" t="s">
+      <c r="G5" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="H5" s="12">
+        <v>3410530510202</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>353</v>
+      </c>
+      <c r="J5" s="23"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="H6" s="12">
+        <v>3546332920458</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>354</v>
+      </c>
+      <c r="J6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="H7" s="12">
+        <v>3410531531206</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="J7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H8" s="12">
+        <v>3410530521307</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="J8" s="23"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="H9" s="12">
+        <v>3546332610250</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="J9" s="23"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="H10" s="12">
+        <v>3546332610496</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="J10" s="23"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H11" s="12">
+        <v>3410531541205</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>360</v>
+      </c>
+      <c r="J11" s="23"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="H12" s="12">
+        <v>3410530231152</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>361</v>
+      </c>
+      <c r="J12" s="23"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="H13" s="12">
+        <v>3661238583740</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>362</v>
+      </c>
+      <c r="J13" s="23"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="H14" s="12">
+        <v>3410530231107</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="J14" s="23"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="H15" s="12">
+        <v>3661238046597</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="J15" s="23"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="H16" s="12">
+        <v>3410531531152</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>365</v>
+      </c>
+      <c r="J16" s="23"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="H17" s="12">
+        <v>3410531543209</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="J17" s="23"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="H18" s="12">
+        <v>3410530231206</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="J18" s="23"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="H19" s="12">
+        <v>3410531543155</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>368</v>
+      </c>
+      <c r="J19" s="23"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="H20" s="12">
+        <v>3661238046580</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>369</v>
+      </c>
+      <c r="J20" s="23"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="H21" s="12">
+        <v>3546332820727</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>370</v>
+      </c>
+      <c r="J21" s="23"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="H22" s="12">
+        <v>3410531544251</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="J22" s="23"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="H23" s="12">
+        <v>3546332820741</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>372</v>
+      </c>
+      <c r="J23" s="23"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="H24" s="12">
+        <v>3546332920311</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="J24" s="23"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="H25" s="12">
+        <v>3410531541151</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>374</v>
+      </c>
+      <c r="J25" s="23"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="H26" s="12">
+        <v>3546332810773</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="J26" s="23"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="H27" s="12">
+        <v>3410530223207</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="J27" s="24"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="H28" s="12">
+        <v>3661238568945</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>377</v>
+      </c>
+      <c r="J28" s="23"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="H29" s="12">
+        <v>3546338714150</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>378</v>
+      </c>
+      <c r="J29" s="23"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="H30" s="12">
+        <v>3410531543254</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>379</v>
+      </c>
+      <c r="J30" s="23"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="H31" s="19">
+        <v>3410530223300</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>380</v>
+      </c>
+      <c r="J31" s="23"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="H32" s="19">
+        <v>3410531531121</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="J32" s="23"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="H33" s="19">
+        <v>3546332310709</v>
+      </c>
+      <c r="I33" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="J33" s="23"/>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="20" t="s">
         <v>337</v>
       </c>
-      <c r="B5" s="13">
-        <f>VLOOKUP(A5,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>11.25</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>335</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>334</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="J5" s="15">
-        <v>3410530510202</v>
-      </c>
-      <c r="K5" s="13">
-        <v>51020</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N5" s="13">
-        <v>621</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P5" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q5" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="B6" s="13">
-        <f>VLOOKUP(A6,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>10.17</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="J6" s="15">
-        <v>3546332920458</v>
-      </c>
-      <c r="K6" s="13">
-        <v>292045</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N6" s="13">
-        <v>621</v>
-      </c>
-      <c r="O6" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P6" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q6" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="B7" s="13">
-        <f>VLOOKUP(A7,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>8.25</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>311</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>310</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="J7" s="15">
-        <v>3410531531206</v>
-      </c>
-      <c r="K7" s="23">
-        <v>153120</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N7" s="23">
-        <v>621</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P7" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q7" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R7" s="14"/>
-      <c r="S7" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="B8" s="13">
-        <f>VLOOKUP(A8,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>7.2</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>330</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>328</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>327</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>326</v>
-      </c>
-      <c r="J8" s="15">
-        <v>3410530521307</v>
-      </c>
-      <c r="K8" s="13">
-        <v>52130</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N8" s="13">
-        <v>621</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P8" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q8" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="B9" s="13">
-        <f>VLOOKUP(A9,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>7.05</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="J9" s="15">
-        <v>3546332610250</v>
-      </c>
-      <c r="K9" s="13">
-        <v>261025</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N9" s="13">
-        <v>621</v>
-      </c>
-      <c r="O9" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P9" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q9" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="B10" s="13">
-        <f>VLOOKUP(A10,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>6.68</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="J10" s="15">
-        <v>3546332610496</v>
-      </c>
-      <c r="K10" s="13">
-        <v>261049</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="M10" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N10" s="13">
-        <v>621</v>
-      </c>
-      <c r="O10" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P10" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q10" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="B11" s="13">
-        <f>VLOOKUP(A11,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>6.06</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>298</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>297</v>
-      </c>
-      <c r="J11" s="15">
-        <v>3410531541205</v>
-      </c>
-      <c r="K11" s="13">
-        <v>154120</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N11" s="13">
-        <v>621</v>
-      </c>
-      <c r="O11" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P11" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q11" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="13" t="s">
+      <c r="B34" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="H34" s="19">
+        <v>3410531531091</v>
+      </c>
+      <c r="I34" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="J34" s="23"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="H35" s="19">
+        <v>3410531531114</v>
+      </c>
+      <c r="I35" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="J35" s="23"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="H36" s="19">
+        <v>3410530211147</v>
+      </c>
+      <c r="I36" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="J36" s="23"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="H37" s="19">
+        <v>3410530510158</v>
+      </c>
+      <c r="I37" s="23" t="s">
+        <v>388</v>
+      </c>
+      <c r="J37" s="23"/>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="20" t="s">
         <v>349</v>
       </c>
-      <c r="B12" s="13">
-        <f>VLOOKUP(A12,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>5.92</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="B38" s="20" t="s">
         <v>348</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="H38" s="19">
+        <v>3410530530170</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>386</v>
+      </c>
+      <c r="J38" s="23"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="21" t="s">
         <v>347</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H12" s="14" t="s">
+      <c r="B39" s="21" t="s">
         <v>345</v>
       </c>
-      <c r="I12" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="J12" s="15">
-        <v>3410530231152</v>
-      </c>
-      <c r="K12" s="13">
-        <v>23115</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N12" s="13">
-        <v>621</v>
-      </c>
-      <c r="O12" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P12" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q12" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B13" s="13">
-        <f>VLOOKUP(A13,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>5.92</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="J13" s="15">
-        <v>3661238583740</v>
-      </c>
-      <c r="K13" s="13">
-        <v>7605044</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N13" s="13">
-        <v>621</v>
-      </c>
-      <c r="O13" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P13" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q13" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="B14" s="13">
-        <f>VLOOKUP(A14,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>4.5</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>352</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>350</v>
-      </c>
-      <c r="J14" s="15">
-        <v>3410530231107</v>
-      </c>
-      <c r="K14" s="13">
-        <v>23110</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N14" s="13">
-        <v>621</v>
-      </c>
-      <c r="O14" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P14" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q14" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="B15" s="13">
-        <f>VLOOKUP(A15,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>4.2</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="J15" s="15">
-        <v>3661238046597</v>
-      </c>
-      <c r="K15" s="13">
-        <v>89789651</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="M15" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N15" s="13">
-        <v>621</v>
-      </c>
-      <c r="O15" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P15" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q15" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="B16" s="13">
-        <f>VLOOKUP(A16,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>3.72</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>318</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>314</v>
-      </c>
-      <c r="J16" s="15">
-        <v>3410531531152</v>
-      </c>
-      <c r="K16" s="13">
-        <v>153115</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M16" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N16" s="13">
-        <v>621</v>
-      </c>
-      <c r="O16" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P16" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q16" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="B17" s="13">
-        <f>VLOOKUP(A17,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>3.67</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="J17" s="15">
-        <v>3410531543209</v>
-      </c>
-      <c r="K17" s="13">
-        <v>154320</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M17" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N17" s="13">
-        <v>621</v>
-      </c>
-      <c r="O17" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P17" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q17" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="13" t="s">
-        <v>343</v>
-      </c>
-      <c r="B18" s="13">
-        <f>VLOOKUP(A18,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>3.58</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="J18" s="15">
-        <v>3410530231206</v>
-      </c>
-      <c r="K18" s="13">
-        <v>23120</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M18" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N18" s="13">
-        <v>621</v>
-      </c>
-      <c r="O18" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P18" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q18" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="7"/>
-      <c r="AA18" s="7"/>
-    </row>
-    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="B19" s="13">
-        <f>VLOOKUP(A19,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>3.03</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="J19" s="15">
-        <v>3410531543155</v>
-      </c>
-      <c r="K19" s="13">
-        <v>154315</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N19" s="13">
-        <v>621</v>
-      </c>
-      <c r="O19" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P19" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q19" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="B20" s="13">
-        <f>VLOOKUP(A20,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="J20" s="15">
-        <v>3661238046580</v>
-      </c>
-      <c r="K20" s="13">
-        <v>89789661</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="M20" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N20" s="13">
-        <v>621</v>
-      </c>
-      <c r="O20" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P20" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q20" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="B21" s="13">
-        <f>VLOOKUP(A21,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>2.8</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>241</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="J21" s="15">
-        <v>3546332820727</v>
-      </c>
-      <c r="K21" s="13">
-        <v>282072</v>
-      </c>
-      <c r="L21" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="M21" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N21" s="13">
-        <v>621</v>
-      </c>
-      <c r="O21" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P21" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q21" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="B22" s="13">
-        <f>VLOOKUP(A22,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>2.77</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="J22" s="15">
-        <v>3410531544251</v>
-      </c>
-      <c r="K22" s="13">
-        <v>154425</v>
-      </c>
-      <c r="L22" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M22" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N22" s="13">
-        <v>621</v>
-      </c>
-      <c r="O22" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P22" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q22" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="B23" s="13">
-        <f>VLOOKUP(A23,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>2.5</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="J23" s="15">
-        <v>3546332820741</v>
-      </c>
-      <c r="K23" s="13">
-        <v>282074</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="M23" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N23" s="13">
-        <v>621</v>
-      </c>
-      <c r="O23" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P23" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q23" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="B24" s="13">
-        <f>VLOOKUP(A24,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>2.33</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="J24" s="15">
-        <v>3546332920311</v>
-      </c>
-      <c r="K24" s="13">
-        <v>292031</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="M24" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N24" s="13">
-        <v>621</v>
-      </c>
-      <c r="O24" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P24" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q24" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="B25" s="13">
-        <f>VLOOKUP(A25,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>305</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="J25" s="15">
-        <v>3410531541151</v>
-      </c>
-      <c r="K25" s="13">
-        <v>154115</v>
-      </c>
-      <c r="L25" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M25" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N25" s="13">
-        <v>621</v>
-      </c>
-      <c r="O25" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P25" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q25" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="B26" s="13">
-        <f>VLOOKUP(A26,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>2.17</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="J26" s="15">
-        <v>3546332810773</v>
-      </c>
-      <c r="K26" s="13">
-        <v>281077</v>
-      </c>
-      <c r="L26" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="M26" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N26" s="13">
-        <v>621</v>
-      </c>
-      <c r="O26" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P26" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q26" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="B27" s="13">
-        <f>VLOOKUP(A27,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>360</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>357</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="J27" s="15">
-        <v>3410530223201</v>
-      </c>
-      <c r="K27" s="13">
-        <v>22120</v>
-      </c>
-      <c r="L27" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M27" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N27" s="13">
-        <v>621</v>
-      </c>
-      <c r="O27" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P27" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q27" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="13" t="s">
-        <v>325</v>
-      </c>
-      <c r="B28" s="13">
-        <f>VLOOKUP(A28,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>324</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>323</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>322</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>321</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="J28" s="15">
-        <v>3661238568945</v>
-      </c>
-      <c r="K28" s="13">
-        <v>100019786</v>
-      </c>
-      <c r="L28" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="M28" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N28" s="13">
-        <v>621</v>
-      </c>
-      <c r="O28" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P28" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q28" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="B29" s="13">
-        <f>VLOOKUP(A29,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="I29" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="J29" s="15">
-        <v>3546338714150</v>
-      </c>
-      <c r="K29" s="13">
-        <v>871415</v>
-      </c>
-      <c r="L29" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="M29" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N29" s="13">
-        <v>621</v>
-      </c>
-      <c r="O29" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P29" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q29" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="B30" s="13">
-        <f>VLOOKUP(A30,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>1.75</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="J30" s="15">
-        <v>3410531543254</v>
-      </c>
-      <c r="K30" s="13">
-        <v>154325</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="M30" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="N30" s="13">
-        <v>621</v>
-      </c>
-      <c r="O30" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="P30" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q30" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+      <c r="H39" s="22">
+        <v>3410530530163</v>
+      </c>
+      <c r="I39" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="J39" s="23"/>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -4327,72 +3634,40 @@
     <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
-  <autoFilter ref="A1:S30" xr:uid="{5F843751-14C2-4F48-A3D1-34202082BFCD}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S30">
-      <sortCondition descending="1" ref="B2:B30"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:H30" xr:uid="{5F843751-14C2-4F48-A3D1-34202082BFCD}"/>
   <hyperlinks>
-    <hyperlink ref="H27" r:id="rId1" xr:uid="{99D8DFD9-6BE7-4C78-ABE2-95EE338B83D8}"/>
-    <hyperlink ref="I27" r:id="rId2" xr:uid="{E3FB3F43-4670-4E99-A48A-D044DBBE2C74}"/>
-    <hyperlink ref="H14" r:id="rId3" xr:uid="{0601F08F-14C2-4EA8-B822-2CDF4698AE78}"/>
-    <hyperlink ref="I14" r:id="rId4" xr:uid="{262CFD04-3ADB-49C9-87CF-82297C1BDE16}"/>
-    <hyperlink ref="H12" r:id="rId5" xr:uid="{F84D323B-A869-4BD4-A35D-2E3C99D524FE}"/>
-    <hyperlink ref="I12" r:id="rId6" xr:uid="{8712264E-1946-426B-8648-27E8AF637FFB}"/>
-    <hyperlink ref="H18" r:id="rId7" xr:uid="{E7FB099C-1EA4-4530-A4CA-0D4044FCC560}"/>
-    <hyperlink ref="I18" r:id="rId8" xr:uid="{ECBD1FE0-91B4-4648-91F4-A13B65EDF8FD}"/>
-    <hyperlink ref="H5" r:id="rId9" xr:uid="{6A74B5BA-8EF1-42D6-9BE6-69B3580C19E3}"/>
-    <hyperlink ref="I5" r:id="rId10" xr:uid="{2048949F-8FAD-4C0F-A0D8-6F2E21D9FF20}"/>
-    <hyperlink ref="H8" r:id="rId11" xr:uid="{B48B8A52-ECB7-4C10-A0FF-0FDB58298CD9}"/>
-    <hyperlink ref="I8" r:id="rId12" xr:uid="{F79786E9-9D1D-4DC5-8BBC-8DC9366FB347}"/>
-    <hyperlink ref="H28" r:id="rId13" xr:uid="{B95B938E-10B4-4A11-8BCA-E6B450153DF1}"/>
-    <hyperlink ref="I28" r:id="rId14" xr:uid="{6C8C2E0F-E162-4F06-A351-9DD2BA1E0116}"/>
-    <hyperlink ref="H16" r:id="rId15" xr:uid="{A02390C4-28A7-4129-A740-C2E37532AAF4}"/>
-    <hyperlink ref="I16" r:id="rId16" xr:uid="{F401772E-4D13-4E69-8345-52BB74433F38}"/>
-    <hyperlink ref="H7" r:id="rId17" xr:uid="{75199553-6D17-44D8-8A66-C4AE2131BD87}"/>
-    <hyperlink ref="I7" r:id="rId18" xr:uid="{890BBFD4-1471-43A2-A056-15E8F736FD4E}"/>
-    <hyperlink ref="H25" r:id="rId19" xr:uid="{2BD9953D-C1E7-4942-A62C-770EEFF28D76}"/>
-    <hyperlink ref="I25" r:id="rId20" xr:uid="{DC634B84-9A48-4EE2-B1F3-5D60C4815BC1}"/>
-    <hyperlink ref="H11" r:id="rId21" xr:uid="{CD963034-D20A-45F7-8273-9009DC597E76}"/>
-    <hyperlink ref="I11" r:id="rId22" xr:uid="{E177113C-5B3C-4A5F-B5E6-E9F6E8FA1B1D}"/>
-    <hyperlink ref="H19" r:id="rId23" xr:uid="{878F7461-702A-47DF-B955-5760FA9EFF1A}"/>
-    <hyperlink ref="I19" r:id="rId24" xr:uid="{BFFC4479-A5D2-420F-9075-6F4C889B61F9}"/>
-    <hyperlink ref="H17" r:id="rId25" xr:uid="{756EB775-EE14-4BBC-9B0C-4E1297FE42D1}"/>
-    <hyperlink ref="I17" r:id="rId26" xr:uid="{8BE6EF28-9646-41BC-8EA5-F8BC8A53BAA8}"/>
-    <hyperlink ref="H30" r:id="rId27" xr:uid="{5F4A6CC3-CCD5-4CF8-B333-8CAFFF58F2B7}"/>
-    <hyperlink ref="I30" r:id="rId28" xr:uid="{00FA8D30-9405-4EDF-9E91-F7F18721DA4B}"/>
-    <hyperlink ref="H2" r:id="rId29" xr:uid="{2A5E8E8C-F0B0-44FD-BAEB-B2C5DAF84D50}"/>
-    <hyperlink ref="I2" r:id="rId30" xr:uid="{D8BBCD78-271C-43B4-8B92-5F7F1E49E4E4}"/>
-    <hyperlink ref="H22" r:id="rId31" xr:uid="{D6FC507A-68E9-4763-AA79-3E87BC9253E8}"/>
-    <hyperlink ref="I22" r:id="rId32" xr:uid="{9A9544DA-4750-4CE1-89AE-F37C5E480315}"/>
-    <hyperlink ref="H3" r:id="rId33" xr:uid="{C9B382F8-D7E2-421C-91EB-8310CF808AB3}"/>
-    <hyperlink ref="I3" r:id="rId34" xr:uid="{8641A7C3-4048-4CDF-ABAD-25A50C9A6EAB}"/>
-    <hyperlink ref="H9" r:id="rId35" xr:uid="{A6B949BA-91A7-4F19-91D9-C27B88A58084}"/>
-    <hyperlink ref="I9" r:id="rId36" xr:uid="{50BCDB5C-AC05-428D-88CE-A9B0CEF73290}"/>
-    <hyperlink ref="H10" r:id="rId37" xr:uid="{ACF0AB68-E7D6-4155-A23A-DCD3B9BB0CDB}"/>
-    <hyperlink ref="I10" r:id="rId38" xr:uid="{B07F25F0-0A89-41A2-A279-5DFA9F5058D5}"/>
-    <hyperlink ref="H26" r:id="rId39" xr:uid="{0A555F60-5921-4BD2-8CB4-E3BF76A23F01}"/>
-    <hyperlink ref="I26" r:id="rId40" xr:uid="{94FB009D-6CB5-4A73-B31C-E7F49070311A}"/>
-    <hyperlink ref="H21" r:id="rId41" xr:uid="{6BF3C264-BD68-4437-8E7C-D84B122C5763}"/>
-    <hyperlink ref="I21" r:id="rId42" xr:uid="{254D2B03-ED1F-4468-B2F0-D1058756198A}"/>
-    <hyperlink ref="H23" r:id="rId43" xr:uid="{541331AF-4CFE-4458-AE54-EE44D847C4FD}"/>
-    <hyperlink ref="I23" r:id="rId44" xr:uid="{79F4E8EE-249E-4920-88BE-07DF6C3B0564}"/>
-    <hyperlink ref="H24" r:id="rId45" xr:uid="{91A7B747-DB67-4060-8560-323DDF1923D2}"/>
-    <hyperlink ref="I24" r:id="rId46" xr:uid="{17074686-B527-478E-836F-3C8EB3B08C9C}"/>
-    <hyperlink ref="H6" r:id="rId47" xr:uid="{F78D3D90-EA33-400F-BE8E-76DBF64142BA}"/>
-    <hyperlink ref="I6" r:id="rId48" xr:uid="{77BB8E84-01A2-4E85-B992-64C45BA2934D}"/>
-    <hyperlink ref="H13" r:id="rId49" xr:uid="{BF64299C-2B33-4D98-A11C-DD41B908AA5B}"/>
-    <hyperlink ref="I13" r:id="rId50" xr:uid="{89324702-ADD1-43D8-9166-3237B9861112}"/>
-    <hyperlink ref="H29" r:id="rId51" xr:uid="{FABCAC6F-0EA0-4D9A-B304-2D38ED3A684A}"/>
-    <hyperlink ref="I29" r:id="rId52" xr:uid="{C7309A15-7EDA-4400-ACAF-2666F1E1193F}"/>
-    <hyperlink ref="H15" r:id="rId53" xr:uid="{73065095-5BFB-47BE-BA84-CF4FF287680D}"/>
-    <hyperlink ref="I15" r:id="rId54" xr:uid="{10E084A1-80B5-4594-BC62-6956C26AB080}"/>
-    <hyperlink ref="H20" r:id="rId55" xr:uid="{BF18D7EE-A205-49E0-807B-B8EDE5723178}"/>
-    <hyperlink ref="I20" r:id="rId56" xr:uid="{B27CCBBD-F8AB-43A7-B92D-9588906D3D87}"/>
+    <hyperlink ref="G27" r:id="rId1" xr:uid="{E3FB3F43-4670-4E99-A48A-D044DBBE2C74}"/>
+    <hyperlink ref="G14" r:id="rId2" xr:uid="{262CFD04-3ADB-49C9-87CF-82297C1BDE16}"/>
+    <hyperlink ref="G12" r:id="rId3" xr:uid="{8712264E-1946-426B-8648-27E8AF637FFB}"/>
+    <hyperlink ref="G18" r:id="rId4" xr:uid="{ECBD1FE0-91B4-4648-91F4-A13B65EDF8FD}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{2048949F-8FAD-4C0F-A0D8-6F2E21D9FF20}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{F79786E9-9D1D-4DC5-8BBC-8DC9366FB347}"/>
+    <hyperlink ref="G28" r:id="rId7" xr:uid="{6C8C2E0F-E162-4F06-A351-9DD2BA1E0116}"/>
+    <hyperlink ref="G16" r:id="rId8" xr:uid="{F401772E-4D13-4E69-8345-52BB74433F38}"/>
+    <hyperlink ref="G7" r:id="rId9" xr:uid="{890BBFD4-1471-43A2-A056-15E8F736FD4E}"/>
+    <hyperlink ref="G25" r:id="rId10" xr:uid="{DC634B84-9A48-4EE2-B1F3-5D60C4815BC1}"/>
+    <hyperlink ref="G11" r:id="rId11" xr:uid="{E177113C-5B3C-4A5F-B5E6-E9F6E8FA1B1D}"/>
+    <hyperlink ref="G19" r:id="rId12" xr:uid="{BFFC4479-A5D2-420F-9075-6F4C889B61F9}"/>
+    <hyperlink ref="G17" r:id="rId13" xr:uid="{8BE6EF28-9646-41BC-8EA5-F8BC8A53BAA8}"/>
+    <hyperlink ref="G30" r:id="rId14" xr:uid="{00FA8D30-9405-4EDF-9E91-F7F18721DA4B}"/>
+    <hyperlink ref="G2" r:id="rId15" xr:uid="{D8BBCD78-271C-43B4-8B92-5F7F1E49E4E4}"/>
+    <hyperlink ref="G22" r:id="rId16" xr:uid="{9A9544DA-4750-4CE1-89AE-F37C5E480315}"/>
+    <hyperlink ref="G3" r:id="rId17" xr:uid="{8641A7C3-4048-4CDF-ABAD-25A50C9A6EAB}"/>
+    <hyperlink ref="G9" r:id="rId18" xr:uid="{50BCDB5C-AC05-428D-88CE-A9B0CEF73290}"/>
+    <hyperlink ref="G10" r:id="rId19" xr:uid="{B07F25F0-0A89-41A2-A279-5DFA9F5058D5}"/>
+    <hyperlink ref="G26" r:id="rId20" xr:uid="{94FB009D-6CB5-4A73-B31C-E7F49070311A}"/>
+    <hyperlink ref="G21" r:id="rId21" xr:uid="{254D2B03-ED1F-4468-B2F0-D1058756198A}"/>
+    <hyperlink ref="G23" r:id="rId22" xr:uid="{79F4E8EE-249E-4920-88BE-07DF6C3B0564}"/>
+    <hyperlink ref="G24" r:id="rId23" xr:uid="{17074686-B527-478E-836F-3C8EB3B08C9C}"/>
+    <hyperlink ref="G6" r:id="rId24" xr:uid="{77BB8E84-01A2-4E85-B992-64C45BA2934D}"/>
+    <hyperlink ref="G13" r:id="rId25" xr:uid="{89324702-ADD1-43D8-9166-3237B9861112}"/>
+    <hyperlink ref="G29" r:id="rId26" xr:uid="{C7309A15-7EDA-4400-ACAF-2666F1E1193F}"/>
+    <hyperlink ref="G15" r:id="rId27" xr:uid="{10E084A1-80B5-4594-BC62-6956C26AB080}"/>
+    <hyperlink ref="G20" r:id="rId28" xr:uid="{B27CCBBD-F8AB-43A7-B92D-9588906D3D87}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" fitToWidth="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+  <pageSetup paperSize="9" fitToWidth="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId29"/>
 </worksheet>
 </file>
 
@@ -4400,9 +3675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FE2415-4BB7-436B-9A78-5295C55F5B91}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>

</xml_diff>